<commit_message>
Support setting complex objects as null
There are a lot of changes here, but most of them are generated, and
there are quite a few for a new end to end test.

The important bit is in SpecificationSpecificClassGenerator where
it uses a "?." instead of a "."
</commit_message>
<xml_diff>
--- a/CustomerTestsExcel.Test/TestExcelFiles/PropertyTypes.xlsx
+++ b/CustomerTestsExcel.Test/TestExcelFiles/PropertyTypes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\Test\TestExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\CustomerTestsExcel.Test\TestExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3AA74B-33C3-4E50-9730-129D4B073726}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0F99DF-FBAC-4844-999A-AD5D5E9ABDE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="AllPropertyTypes" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>DateTime of</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>StringNull of</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>"1"</t>
+  </si>
+  <si>
+    <t>"null"</t>
   </si>
 </sst>
 </file>
@@ -567,23 +567,23 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -599,25 +599,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
@@ -625,78 +625,78 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C9" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add codecov changes recommended by codecov team
</commit_message>
<xml_diff>
--- a/CustomerTestsExcel.Test/TestExcelFiles/PropertyTypes.xlsx
+++ b/CustomerTestsExcel.Test/TestExcelFiles/PropertyTypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\CustomerTestsExcel.Test\TestExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0F99DF-FBAC-4844-999A-AD5D5E9ABDE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872BE396-9823-49F3-B762-ABF874D4F4A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11265" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="AllPropertyTypes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Specification</t>
   </si>
@@ -39,9 +39,6 @@
     <t>When</t>
   </si>
   <si>
-    <t>Assert</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
@@ -103,6 +100,12 @@
   </si>
   <si>
     <t>"null"</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Then</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +591,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,20 +609,23 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2">
         <v>43466</v>
@@ -627,15 +633,15 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -643,15 +649,15 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="b">
         <v>0</v>
@@ -659,7 +665,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="b">
         <v>1</v>
@@ -667,18 +673,18 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,23 +692,23 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove StringNull enum option
This was always a bin pointless and just created extra conditionals,
but it also didn't work with the recent change in GivenClassMutable
</commit_message>
<xml_diff>
--- a/CustomerTestsExcel.Test/TestExcelFiles/PropertyTypes.xlsx
+++ b/CustomerTestsExcel.Test/TestExcelFiles/PropertyTypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\CustomerTestsExcel.Test\TestExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872BE396-9823-49F3-B762-ABF874D4F4A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D4ED24-50D1-4EDB-8DDA-14485FE5102D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11265" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="AllPropertyTypes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Specification</t>
   </si>
@@ -57,9 +57,6 @@
     <t>DateTime of</t>
   </si>
   <si>
-    <t>StringNull of</t>
-  </si>
-  <si>
     <t>Enum of</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
   </si>
   <si>
     <t>"1"</t>
-  </si>
-  <si>
-    <t>"null"</t>
   </si>
   <si>
     <t>null</t>
@@ -567,26 +561,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1389079D-C9FD-4AFA-AFB3-2F9AFFAD165C}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -602,112 +596,104 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>43466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2">
-        <v>43466</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>